<commit_message>
display loss curves and accuracy curves
</commit_message>
<xml_diff>
--- a/movinet_loss_curves.xlsx
+++ b/movinet_loss_curves.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df9d8495cd692d4a/echonet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC51876D-D444-4590-B92A-8DFED729FB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{DC51876D-D444-4590-B92A-8DFED729FB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30642E39-4212-4A20-A9EC-6BD1151AF52A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{98BF7866-0A29-4E70-AC44-51CA9B5E8988}"/>
   </bookViews>
   <sheets>
     <sheet name="A0-mod-rEF" sheetId="3" r:id="rId1"/>
-    <sheet name="A0-sem-rEF" sheetId="6" r:id="rId2"/>
-    <sheet name="A0-ext-rEF" sheetId="1" r:id="rId3"/>
-    <sheet name="A1-mod-rEF" sheetId="2" r:id="rId4"/>
-    <sheet name="A1-ext-rEF" sheetId="5" r:id="rId5"/>
-    <sheet name="A0-mod-npEF" sheetId="7" r:id="rId6"/>
-    <sheet name="A0-ext-npEF" sheetId="8" r:id="rId7"/>
+    <sheet name="A0-ext-rEF" sheetId="1" r:id="rId2"/>
+    <sheet name="A1-mod-rEF" sheetId="2" r:id="rId3"/>
+    <sheet name="A1-ext-rEF" sheetId="5" r:id="rId4"/>
+    <sheet name="A0-mod-npEF" sheetId="7" r:id="rId5"/>
+    <sheet name="A0-ext-npEF" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="138">
   <si>
     <t xml:space="preserve">Phase: train Epoch: 1/10 Loss: 0.6160 Acc: 0.6420        </t>
   </si>
@@ -321,72 +320,6 @@
   </si>
   <si>
     <t>Best test loss: 0.4164 | Best test accuracy: 0.7664</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: train Epoch: 1/10 Loss: 0.5877 Acc: 0.6742        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: val Epoch: 1/10 Loss: 0.4535 Acc: 0.7150        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: train Epoch: 2/10 Loss: 0.4841 Acc: 0.7570        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: val Epoch: 2/10 Loss: 0.4203 Acc: 0.7290        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: train Epoch: 3/10 Loss: 0.4378 Acc: 0.7916        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: val Epoch: 3/10 Loss: 0.4180 Acc: 0.7430        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: train Epoch: 4/10 Loss: 0.4130 Acc: 0.8077        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: val Epoch: 4/10 Loss: 0.4282 Acc: 0.7570        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: train Epoch: 5/10 Loss: 0.3944 Acc: 0.8182        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: val Epoch: 5/10 Loss: 0.4395 Acc: 0.7617        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: train Epoch: 6/10 Loss: 0.3776 Acc: 0.8286        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: val Epoch: 6/10 Loss: 0.4538 Acc: 0.7477        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: train Epoch: 7/10 Loss: 0.3676 Acc: 0.8343        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: val Epoch: 7/10 Loss: 0.4657 Acc: 0.7570        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: train Epoch: 8/10 Loss: 0.3530 Acc: 0.8399        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: val Epoch: 8/10 Loss: 0.4772 Acc: 0.7523        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: train Epoch: 9/10 Loss: 0.3388 Acc: 0.8528        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: val Epoch: 9/10 Loss: 0.4888 Acc: 0.7477        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: train Epoch: 10/10 Loss: 0.3311 Acc: 0.8544        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase: val Epoch: 10/10 Loss: 0.5199 Acc: 0.7196        </t>
-  </si>
-  <si>
-    <t>Training completed in 312m 25s</t>
-  </si>
-  <si>
-    <t>Best test loss: 0.4180 | Best test accuracy: 0.7617</t>
   </si>
   <si>
     <t>Phase: train Epoch: 1/10 Loss: 0.6181 Acc: 0.6848        1</t>
@@ -1251,7 +1184,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A1-ext-rEF'!$K$1</c:f>
+              <c:f>'A0-mod-npEF'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1286,39 +1219,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'A1-ext-rEF'!$K$2:$K$11</c:f>
+              <c:f>'A0-mod-npEF'!$K$2:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.6573</c:v>
+                  <c:v>0.68479999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7369</c:v>
+                  <c:v>0.73070000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75619999999999998</c:v>
+                  <c:v>0.75319999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76990000000000003</c:v>
+                  <c:v>0.75970000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.77229999999999999</c:v>
+                  <c:v>0.76490000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.77390000000000003</c:v>
+                  <c:v>0.76970000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.78839999999999999</c:v>
+                  <c:v>0.77400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.78280000000000005</c:v>
+                  <c:v>0.7732</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.78439999999999999</c:v>
+                  <c:v>0.77490000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.78120000000000001</c:v>
+                  <c:v>0.77710000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1326,7 +1259,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DA81-44EF-81B6-C5E674FE5311}"/>
+              <c16:uniqueId val="{00000000-455A-40C2-8CF0-20B696DF3CDF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1335,7 +1268,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A1-ext-rEF'!$L$1</c:f>
+              <c:f>'A0-mod-npEF'!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1370,39 +1303,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'A1-ext-rEF'!$L$2:$L$11</c:f>
+              <c:f>'A0-mod-npEF'!$L$2:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.67759999999999998</c:v>
+                  <c:v>0.71499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71499999999999997</c:v>
+                  <c:v>0.72799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73360000000000003</c:v>
+                  <c:v>0.73829999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.72430000000000005</c:v>
+                  <c:v>0.73829999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.72899999999999998</c:v>
+                  <c:v>0.73829999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.71499999999999997</c:v>
+                  <c:v>0.7409</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.71960000000000002</c:v>
+                  <c:v>0.74609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.71030000000000004</c:v>
+                  <c:v>0.74350000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.69159999999999999</c:v>
+                  <c:v>0.74870000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.69159999999999999</c:v>
+                  <c:v>0.75129999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1410,7 +1343,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DA81-44EF-81B6-C5E674FE5311}"/>
+              <c16:uniqueId val="{00000001-455A-40C2-8CF0-20B696DF3CDF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1764,1145 +1697,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>MoViNet A0 modified</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'A0-mod-npEF'!$S$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>train</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'A0-mod-npEF'!$R$2:$R$11</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'A0-mod-npEF'!$S$2:$S$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.61809999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.54949999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.51970000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.502</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.49059999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.4824</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.47449999999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.46860000000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.4627</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.45950000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E310-43CC-82B5-60DA3DDA5359}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'A0-mod-npEF'!$T$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>val</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'A0-mod-npEF'!$R$2:$R$11</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'A0-mod-npEF'!$T$2:$T$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.56210000000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.52739999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.51039999999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.49969999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.49340000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.48899999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.48620000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.48199999999999998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.47939999999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.47799999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E310-43CC-82B5-60DA3DDA5359}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="771622752"/>
-        <c:axId val="771623832"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="771622752"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Epoch</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="771623832"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="771623832"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="0.70000000000000007"/>
-          <c:min val="0.4"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Loss</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="771622752"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1200"/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'A0-mod-npEF'!$K$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>train</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'A0-mod-npEF'!$K$2:$K$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.68479999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.73070000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.75319999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.75970000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.76490000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.76970000000000005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.77400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.7732</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.77490000000000003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.77710000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-455A-40C2-8CF0-20B696DF3CDF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'A0-mod-npEF'!$L$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>val</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'A0-mod-npEF'!$L$2:$L$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.71499999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.72799999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.73829999999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.73829999999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.73829999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.7409</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.74609999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.74350000000000005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.74870000000000003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.75129999999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-455A-40C2-8CF0-20B696DF3CDF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="771622752"/>
-        <c:axId val="771623832"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="771622752"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Epoch</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="771623832"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="771623832"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="0.9"/>
-          <c:min val="0.60000000000000009"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Accuracy</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="771622752"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1200"/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>MoViNet A0 extended</a:t>
             </a:r>
           </a:p>
@@ -3504,7 +2298,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4545,7 +3339,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>MoViNet A0 "semifreddo"</a:t>
+              <a:t>MoViNet A0 extended</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4590,7 +3384,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A0-sem-rEF'!$S$1</c:f>
+              <c:f>'A0-ext-rEF'!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4625,7 +3419,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'A0-sem-rEF'!$R$2:$R$11</c:f>
+              <c:f>'A0-ext-rEF'!$R$2:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4664,39 +3458,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'A0-sem-rEF'!$S$2:$S$11</c:f>
+              <c:f>'A0-ext-rEF'!$S$2:$S$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.5877</c:v>
+                  <c:v>0.61599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.48409999999999997</c:v>
+                  <c:v>0.51090000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.43780000000000002</c:v>
+                  <c:v>0.48170000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41299999999999998</c:v>
+                  <c:v>0.46899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.39439999999999997</c:v>
+                  <c:v>0.45529999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.37759999999999999</c:v>
+                  <c:v>0.44519999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36759999999999998</c:v>
+                  <c:v>0.44669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.35299999999999998</c:v>
+                  <c:v>0.43709999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33879999999999999</c:v>
+                  <c:v>0.433</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33110000000000001</c:v>
+                  <c:v>0.41270000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4704,7 +3498,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A5FE-471C-A1E0-4C3931DECC34}"/>
+              <c16:uniqueId val="{00000001-4249-4339-9588-4FA3C1F89C22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4713,7 +3507,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A0-sem-rEF'!$T$1</c:f>
+              <c:f>'A0-ext-rEF'!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4748,7 +3542,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'A0-sem-rEF'!$R$2:$R$11</c:f>
+              <c:f>'A0-ext-rEF'!$R$2:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4787,39 +3581,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'A0-sem-rEF'!$T$2:$T$11</c:f>
+              <c:f>'A0-ext-rEF'!$T$2:$T$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.45350000000000001</c:v>
+                  <c:v>0.46810000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42030000000000001</c:v>
+                  <c:v>0.44259999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.41799999999999998</c:v>
+                  <c:v>0.4325</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42820000000000003</c:v>
+                  <c:v>0.43109999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4395</c:v>
+                  <c:v>0.43219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.45379999999999998</c:v>
+                  <c:v>0.436</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.4657</c:v>
+                  <c:v>0.4471</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.47720000000000001</c:v>
+                  <c:v>0.441</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.48880000000000001</c:v>
+                  <c:v>0.441</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.51990000000000003</c:v>
+                  <c:v>0.44209999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4827,7 +3621,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A5FE-471C-A1E0-4C3931DECC34}"/>
+              <c16:uniqueId val="{00000002-4249-4339-9588-4FA3C1F89C22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4954,8 +3748,8 @@
         <c:axId val="771623832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.60000000000000009"/>
-          <c:min val="0.30000000000000004"/>
+          <c:max val="0.70000000000000007"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5171,7 +3965,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A0-sem-rEF'!$K$1</c:f>
+              <c:f>'A0-ext-rEF'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5206,39 +4000,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'A0-sem-rEF'!$K$2:$K$11</c:f>
+              <c:f>'A0-ext-rEF'!$K$2:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.67420000000000002</c:v>
+                  <c:v>0.64200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75700000000000001</c:v>
+                  <c:v>0.74009999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.79159999999999997</c:v>
+                  <c:v>0.7651</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.80769999999999997</c:v>
+                  <c:v>0.77470000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81820000000000004</c:v>
+                  <c:v>0.78439999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8286</c:v>
+                  <c:v>0.78839999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.83430000000000004</c:v>
+                  <c:v>0.78520000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.83989999999999998</c:v>
+                  <c:v>0.79239999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8528</c:v>
+                  <c:v>0.79320000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.85440000000000005</c:v>
+                  <c:v>0.81740000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5246,7 +4040,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9589-4DD3-95A5-ABAA712650A9}"/>
+              <c16:uniqueId val="{00000002-499F-4398-BA0C-BD5E3148A1B2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5255,7 +4049,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A0-sem-rEF'!$L$1</c:f>
+              <c:f>'A0-ext-rEF'!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5290,7 +4084,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'A0-sem-rEF'!$L$2:$L$11</c:f>
+              <c:f>'A0-ext-rEF'!$L$2:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5298,31 +4092,31 @@
                   <c:v>0.71499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.71960000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.72899999999999998</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.73360000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73360000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.73360000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73360000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74770000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.74299999999999999</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.75700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.76170000000000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.74770000000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.75700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.75229999999999997</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.74770000000000003</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.71960000000000002</c:v>
+                  <c:v>0.72430000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5330,7 +4124,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9589-4DD3-95A5-ABAA712650A9}"/>
+              <c16:uniqueId val="{00000003-499F-4398-BA0C-BD5E3148A1B2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5684,7 +4478,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>MoViNet A0 extended</a:t>
+              <a:t>MoViNet A1 modified</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5729,7 +4523,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A0-ext-rEF'!$S$1</c:f>
+              <c:f>'A1-mod-rEF'!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5764,7 +4558,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'A0-ext-rEF'!$R$2:$R$11</c:f>
+              <c:f>'A1-mod-rEF'!$R$2:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5803,39 +4597,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'A0-ext-rEF'!$S$2:$S$11</c:f>
+              <c:f>'A1-mod-rEF'!$S$2:$S$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.61599999999999999</c:v>
+                  <c:v>0.66010000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51090000000000002</c:v>
+                  <c:v>0.60240000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.48170000000000002</c:v>
+                  <c:v>0.56669999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46899999999999997</c:v>
+                  <c:v>0.54279999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45529999999999998</c:v>
+                  <c:v>0.52480000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.44519999999999998</c:v>
+                  <c:v>0.51049999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.44669999999999999</c:v>
+                  <c:v>0.50019999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.43709999999999999</c:v>
+                  <c:v>0.48970000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.433</c:v>
+                  <c:v>0.48099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.41270000000000001</c:v>
+                  <c:v>0.4738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5843,7 +4637,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4249-4339-9588-4FA3C1F89C22}"/>
+              <c16:uniqueId val="{00000000-0054-4887-9A87-4C3CBB995AE9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5852,7 +4646,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A0-ext-rEF'!$T$1</c:f>
+              <c:f>'A1-mod-rEF'!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5887,7 +4681,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'A0-ext-rEF'!$R$2:$R$11</c:f>
+              <c:f>'A1-mod-rEF'!$R$2:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5926,39 +4720,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'A0-ext-rEF'!$T$2:$T$11</c:f>
+              <c:f>'A1-mod-rEF'!$T$2:$T$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.46810000000000002</c:v>
+                  <c:v>0.58030000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44259999999999999</c:v>
+                  <c:v>0.53859999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4325</c:v>
+                  <c:v>0.51339999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.43109999999999998</c:v>
+                  <c:v>0.49709999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43219999999999997</c:v>
+                  <c:v>0.48580000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.436</c:v>
+                  <c:v>0.4773</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.4471</c:v>
+                  <c:v>0.4708</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.441</c:v>
+                  <c:v>0.46560000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.441</c:v>
+                  <c:v>0.46129999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44209999999999999</c:v>
+                  <c:v>0.45879999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5966,7 +4760,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4249-4339-9588-4FA3C1F89C22}"/>
+              <c16:uniqueId val="{00000001-0054-4887-9A87-4C3CBB995AE9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6310,7 +5104,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A0-ext-rEF'!$K$1</c:f>
+              <c:f>'A1-mod-rEF'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6345,39 +5139,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'A0-ext-rEF'!$K$2:$K$11</c:f>
+              <c:f>'A1-mod-rEF'!$K$2:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.64200000000000002</c:v>
+                  <c:v>0.66290000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.74009999999999998</c:v>
+                  <c:v>0.73529999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7651</c:v>
+                  <c:v>0.75219999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.77470000000000006</c:v>
+                  <c:v>0.76349999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78439999999999999</c:v>
+                  <c:v>0.76029999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.78839999999999999</c:v>
+                  <c:v>0.76749999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.78520000000000001</c:v>
+                  <c:v>0.76829999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.79239999999999999</c:v>
+                  <c:v>0.78120000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79320000000000002</c:v>
+                  <c:v>0.7772</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.81740000000000002</c:v>
+                  <c:v>0.78200000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6385,7 +5179,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-499F-4398-BA0C-BD5E3148A1B2}"/>
+              <c16:uniqueId val="{00000000-94DF-4A38-A9AC-EF0F53E2E77E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6394,7 +5188,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A0-ext-rEF'!$L$1</c:f>
+              <c:f>'A1-mod-rEF'!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6429,39 +5223,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'A0-ext-rEF'!$L$2:$L$11</c:f>
+              <c:f>'A1-mod-rEF'!$L$2:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.67759999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69159999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70089999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.71499999999999997</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.71960000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.72899999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.73360000000000003</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.73360000000000003</c:v>
+                  <c:v>0.71499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.73360000000000003</c:v>
+                  <c:v>0.69630000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73360000000000003</c:v>
+                  <c:v>0.69159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.74770000000000003</c:v>
+                  <c:v>0.68689999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.74299999999999999</c:v>
+                  <c:v>0.69159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.72430000000000005</c:v>
+                  <c:v>0.69159999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6469,7 +5263,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-499F-4398-BA0C-BD5E3148A1B2}"/>
+              <c16:uniqueId val="{00000001-94DF-4A38-A9AC-EF0F53E2E77E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6823,7 +5617,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>MoViNet A1 modified</a:t>
+              <a:t>MoViNet A1 extended</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6868,7 +5662,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A1-mod-rEF'!$S$1</c:f>
+              <c:f>'A1-ext-rEF'!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6903,7 +5697,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'A1-mod-rEF'!$R$2:$R$11</c:f>
+              <c:f>'A1-ext-rEF'!$R$2:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6942,39 +5736,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'A1-mod-rEF'!$S$2:$S$11</c:f>
+              <c:f>'A1-ext-rEF'!$S$2:$S$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.66010000000000002</c:v>
+                  <c:v>0.60780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60240000000000005</c:v>
+                  <c:v>0.52029999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56669999999999998</c:v>
+                  <c:v>0.4904</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.54279999999999995</c:v>
+                  <c:v>0.47820000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.52480000000000004</c:v>
+                  <c:v>0.46460000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51049999999999995</c:v>
+                  <c:v>0.4551</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.50019999999999998</c:v>
+                  <c:v>0.44490000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.48970000000000002</c:v>
+                  <c:v>0.44790000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.48099999999999998</c:v>
+                  <c:v>0.44040000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.4738</c:v>
+                  <c:v>0.43090000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6982,7 +5776,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0054-4887-9A87-4C3CBB995AE9}"/>
+              <c16:uniqueId val="{00000000-262F-4A08-B50C-0E482BF108AD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6991,7 +5785,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A1-mod-rEF'!$T$1</c:f>
+              <c:f>'A1-ext-rEF'!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7026,7 +5820,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'A1-mod-rEF'!$R$2:$R$11</c:f>
+              <c:f>'A1-ext-rEF'!$R$2:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7065,39 +5859,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'A1-mod-rEF'!$T$2:$T$11</c:f>
+              <c:f>'A1-ext-rEF'!$T$2:$T$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.58030000000000004</c:v>
+                  <c:v>0.4738</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53859999999999997</c:v>
+                  <c:v>0.45619999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.51339999999999997</c:v>
+                  <c:v>0.45250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.49709999999999999</c:v>
+                  <c:v>0.4536</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.48580000000000001</c:v>
+                  <c:v>0.4572</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4773</c:v>
+                  <c:v>0.46360000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.4708</c:v>
+                  <c:v>0.46829999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.46560000000000001</c:v>
+                  <c:v>0.47170000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.46129999999999999</c:v>
+                  <c:v>0.47670000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45879999999999999</c:v>
+                  <c:v>0.48309999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7105,7 +5899,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0054-4887-9A87-4C3CBB995AE9}"/>
+              <c16:uniqueId val="{00000001-262F-4A08-B50C-0E482BF108AD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7449,7 +6243,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A1-mod-rEF'!$K$1</c:f>
+              <c:f>'A1-ext-rEF'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7484,39 +6278,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'A1-mod-rEF'!$K$2:$K$11</c:f>
+              <c:f>'A1-ext-rEF'!$K$2:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.66290000000000004</c:v>
+                  <c:v>0.6573</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73529999999999995</c:v>
+                  <c:v>0.7369</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75219999999999998</c:v>
+                  <c:v>0.75619999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76349999999999996</c:v>
+                  <c:v>0.76990000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.76029999999999998</c:v>
+                  <c:v>0.77229999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76749999999999996</c:v>
+                  <c:v>0.77390000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.76829999999999998</c:v>
+                  <c:v>0.78839999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.78280000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78439999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.78120000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.7772</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.78200000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7524,7 +6318,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-94DF-4A38-A9AC-EF0F53E2E77E}"/>
+              <c16:uniqueId val="{00000000-DA81-44EF-81B6-C5E674FE5311}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7533,7 +6327,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A1-mod-rEF'!$L$1</c:f>
+              <c:f>'A1-ext-rEF'!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7568,7 +6362,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'A1-mod-rEF'!$L$2:$L$11</c:f>
+              <c:f>'A1-ext-rEF'!$L$2:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7576,25 +6370,25 @@
                   <c:v>0.67759999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69159999999999999</c:v>
+                  <c:v>0.71499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70089999999999997</c:v>
+                  <c:v>0.73360000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.72430000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.71499999999999997</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.71499999999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69630000000000003</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.69159999999999999</c:v>
+                  <c:v>0.71960000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68689999999999996</c:v>
+                  <c:v>0.71030000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.69159999999999999</c:v>
@@ -7608,7 +6402,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-94DF-4A38-A9AC-EF0F53E2E77E}"/>
+              <c16:uniqueId val="{00000001-DA81-44EF-81B6-C5E674FE5311}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7962,7 +6756,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>MoViNet A1 extended</a:t>
+              <a:t>MoViNet A0 modified</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -8007,7 +6801,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A1-ext-rEF'!$S$1</c:f>
+              <c:f>'A0-mod-npEF'!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8042,7 +6836,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'A1-ext-rEF'!$R$2:$R$11</c:f>
+              <c:f>'A0-mod-npEF'!$R$2:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8081,39 +6875,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'A1-ext-rEF'!$S$2:$S$11</c:f>
+              <c:f>'A0-mod-npEF'!$S$2:$S$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.60780000000000001</c:v>
+                  <c:v>0.61809999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.52029999999999998</c:v>
+                  <c:v>0.54949999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4904</c:v>
+                  <c:v>0.51970000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47820000000000001</c:v>
+                  <c:v>0.502</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46460000000000001</c:v>
+                  <c:v>0.49059999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4551</c:v>
+                  <c:v>0.4824</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.44490000000000002</c:v>
+                  <c:v>0.47449999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.44790000000000002</c:v>
+                  <c:v>0.46860000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.44040000000000001</c:v>
+                  <c:v>0.4627</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.43090000000000001</c:v>
+                  <c:v>0.45950000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8121,7 +6915,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-262F-4A08-B50C-0E482BF108AD}"/>
+              <c16:uniqueId val="{00000000-E310-43CC-82B5-60DA3DDA5359}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8130,7 +6924,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'A1-ext-rEF'!$T$1</c:f>
+              <c:f>'A0-mod-npEF'!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8165,7 +6959,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'A1-ext-rEF'!$R$2:$R$11</c:f>
+              <c:f>'A0-mod-npEF'!$R$2:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8204,39 +6998,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'A1-ext-rEF'!$T$2:$T$11</c:f>
+              <c:f>'A0-mod-npEF'!$T$2:$T$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.4738</c:v>
+                  <c:v>0.56210000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.45619999999999999</c:v>
+                  <c:v>0.52739999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45250000000000001</c:v>
+                  <c:v>0.51039999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4536</c:v>
+                  <c:v>0.49969999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4572</c:v>
+                  <c:v>0.49340000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46360000000000001</c:v>
+                  <c:v>0.48899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46829999999999999</c:v>
+                  <c:v>0.48620000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.47170000000000001</c:v>
+                  <c:v>0.48199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.47670000000000001</c:v>
+                  <c:v>0.47939999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.48309999999999997</c:v>
+                  <c:v>0.47799999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8244,7 +7038,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-262F-4A08-B50C-0E482BF108AD}"/>
+              <c16:uniqueId val="{00000001-E310-43CC-82B5-60DA3DDA5359}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8723,86 +7517,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -11135,1012 +9849,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -16263,87 +13971,6 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46F2A0AB-E7A2-4AC7-8FDC-CB1AE01898EF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC063779-47F1-43A6-A469-D17A12E50CFA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
@@ -16406,7 +14033,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -16487,7 +14114,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -16568,7 +14195,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -16649,7 +14276,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -17826,790 +15453,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3BE197B-6580-4907-B149-631086C9CA7B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0F3B07-AAFA-46F0-8254-5693D6AC1D0A}">
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="7" max="8" width="9.140625" style="2"/>
-    <col min="10" max="10" width="9.140625" style="4"/>
-    <col min="11" max="12" width="9.140625" style="3"/>
-    <col min="18" max="18" width="9.140625" style="4"/>
-    <col min="19" max="20" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20">
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="2" t="str">
-        <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(A2,":",-1)," ",-1)</f>
-        <v xml:space="preserve"> 0.6742       </v>
-      </c>
-      <c r="H2" s="2" t="str">
-        <f>G2</f>
-        <v xml:space="preserve"> 0.6742       </v>
-      </c>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3">
-        <f>_xlfn.NUMBERVALUE(H2,".")/10000</f>
-        <v>0.67420000000000002</v>
-      </c>
-      <c r="L2" s="3">
-        <f>_xlfn.NUMBERVALUE(I12,".")/10000</f>
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="N2" t="str">
-        <f>_xlfn.TEXTAFTER(A2,":",-2)</f>
-        <v xml:space="preserve"> 0.5877 Acc: 0.6742        </v>
-      </c>
-      <c r="O2" t="str">
-        <f>_xlfn.TEXTBEFORE(N2," Acc",-1)</f>
-        <v xml:space="preserve"> 0.5877</v>
-      </c>
-      <c r="P2" s="2" t="str">
-        <f>O2</f>
-        <v xml:space="preserve"> 0.5877</v>
-      </c>
-      <c r="R2" s="4">
-        <v>1</v>
-      </c>
-      <c r="S2" s="3">
-        <f>_xlfn.NUMBERVALUE(P2,".")/10000</f>
-        <v>0.5877</v>
-      </c>
-      <c r="T2" s="3">
-        <f>_xlfn.NUMBERVALUE(Q12,".")/10000</f>
-        <v>0.45350000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="2" t="str">
-        <f t="shared" ref="G3:G21" si="0">_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(A3,":",-1)," ",-1)</f>
-        <v xml:space="preserve"> 0.7150       </v>
-      </c>
-      <c r="H3" s="2" t="str">
-        <f>G4</f>
-        <v xml:space="preserve"> 0.7570       </v>
-      </c>
-      <c r="J3" s="4">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3">
-        <f t="shared" ref="K3:K11" si="1">_xlfn.NUMBERVALUE(H3,".")/10000</f>
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="L3" s="3">
-        <f t="shared" ref="L3:L11" si="2">_xlfn.NUMBERVALUE(I13,".")/10000</f>
-        <v>0.72899999999999998</v>
-      </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:N21" si="3">_xlfn.TEXTAFTER(A3,":",-2)</f>
-        <v xml:space="preserve"> 0.4535 Acc: 0.7150        </v>
-      </c>
-      <c r="O3" t="str">
-        <f t="shared" ref="O3:O21" si="4">_xlfn.TEXTBEFORE(N3," Acc",-1)</f>
-        <v xml:space="preserve"> 0.4535</v>
-      </c>
-      <c r="P3" s="2" t="str">
-        <f>O4</f>
-        <v xml:space="preserve"> 0.4841</v>
-      </c>
-      <c r="R3" s="4">
-        <v>2</v>
-      </c>
-      <c r="S3" s="3">
-        <f t="shared" ref="S3:S11" si="5">_xlfn.NUMBERVALUE(P3,".")/10000</f>
-        <v>0.48409999999999997</v>
-      </c>
-      <c r="T3" s="3">
-        <f t="shared" ref="T3:T11" si="6">_xlfn.NUMBERVALUE(Q13,".")/10000</f>
-        <v>0.42030000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7570       </v>
-      </c>
-      <c r="H4" s="2" t="str">
-        <f>G6</f>
-        <v xml:space="preserve"> 0.7916       </v>
-      </c>
-      <c r="J4" s="4">
-        <v>3</v>
-      </c>
-      <c r="K4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.79159999999999997</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="2"/>
-        <v>0.74299999999999999</v>
-      </c>
-      <c r="N4" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4841 Acc: 0.7570        </v>
-      </c>
-      <c r="O4" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4841</v>
-      </c>
-      <c r="P4" s="2" t="str">
-        <f>O6</f>
-        <v xml:space="preserve"> 0.4378</v>
-      </c>
-      <c r="R4" s="4">
-        <v>3</v>
-      </c>
-      <c r="S4" s="3">
-        <f t="shared" si="5"/>
-        <v>0.43780000000000002</v>
-      </c>
-      <c r="T4" s="3">
-        <f t="shared" si="6"/>
-        <v>0.41799999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7290       </v>
-      </c>
-      <c r="H5" s="2" t="str">
-        <f>G8</f>
-        <v xml:space="preserve"> 0.8077       </v>
-      </c>
-      <c r="J5" s="4">
-        <v>4</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.80769999999999997</v>
-      </c>
-      <c r="L5" s="3">
-        <f t="shared" si="2"/>
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="N5" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4203 Acc: 0.7290        </v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4203</v>
-      </c>
-      <c r="P5" s="2" t="str">
-        <f>O8</f>
-        <v xml:space="preserve"> 0.4130</v>
-      </c>
-      <c r="R5" s="4">
-        <v>4</v>
-      </c>
-      <c r="S5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.41299999999999998</v>
-      </c>
-      <c r="T5" s="3">
-        <f t="shared" si="6"/>
-        <v>0.42820000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7916       </v>
-      </c>
-      <c r="H6" s="2" t="str">
-        <f>G10</f>
-        <v xml:space="preserve"> 0.8182       </v>
-      </c>
-      <c r="J6" s="4">
-        <v>5</v>
-      </c>
-      <c r="K6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.81820000000000004</v>
-      </c>
-      <c r="L6" s="3">
-        <f t="shared" si="2"/>
-        <v>0.76170000000000004</v>
-      </c>
-      <c r="N6" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4378 Acc: 0.7916        </v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4378</v>
-      </c>
-      <c r="P6" s="2" t="str">
-        <f>O10</f>
-        <v xml:space="preserve"> 0.3944</v>
-      </c>
-      <c r="R6" s="4">
-        <v>5</v>
-      </c>
-      <c r="S6" s="3">
-        <f t="shared" si="5"/>
-        <v>0.39439999999999997</v>
-      </c>
-      <c r="T6" s="3">
-        <f t="shared" si="6"/>
-        <v>0.4395</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7430       </v>
-      </c>
-      <c r="H7" s="2" t="str">
-        <f>G12</f>
-        <v xml:space="preserve"> 0.8286       </v>
-      </c>
-      <c r="J7" s="4">
-        <v>6</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.8286</v>
-      </c>
-      <c r="L7" s="3">
-        <f t="shared" si="2"/>
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4180 Acc: 0.7430        </v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4180</v>
-      </c>
-      <c r="P7" s="2" t="str">
-        <f>O12</f>
-        <v xml:space="preserve"> 0.3776</v>
-      </c>
-      <c r="R7" s="4">
-        <v>6</v>
-      </c>
-      <c r="S7" s="3">
-        <f t="shared" si="5"/>
-        <v>0.37759999999999999</v>
-      </c>
-      <c r="T7" s="3">
-        <f t="shared" si="6"/>
-        <v>0.45379999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.8077       </v>
-      </c>
-      <c r="H8" s="2" t="str">
-        <f>G14</f>
-        <v xml:space="preserve"> 0.8343       </v>
-      </c>
-      <c r="J8" s="4">
-        <v>7</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" si="1"/>
-        <v>0.83430000000000004</v>
-      </c>
-      <c r="L8" s="3">
-        <f t="shared" si="2"/>
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="N8" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4130 Acc: 0.8077        </v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4130</v>
-      </c>
-      <c r="P8" s="2" t="str">
-        <f>O14</f>
-        <v xml:space="preserve"> 0.3676</v>
-      </c>
-      <c r="R8" s="4">
-        <v>7</v>
-      </c>
-      <c r="S8" s="3">
-        <f t="shared" si="5"/>
-        <v>0.36759999999999998</v>
-      </c>
-      <c r="T8" s="3">
-        <f t="shared" si="6"/>
-        <v>0.4657</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7570       </v>
-      </c>
-      <c r="H9" s="2" t="str">
-        <f>G16</f>
-        <v xml:space="preserve"> 0.8399       </v>
-      </c>
-      <c r="J9" s="4">
-        <v>8</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="1"/>
-        <v>0.83989999999999998</v>
-      </c>
-      <c r="L9" s="3">
-        <f t="shared" si="2"/>
-        <v>0.75229999999999997</v>
-      </c>
-      <c r="N9" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4282 Acc: 0.7570        </v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4282</v>
-      </c>
-      <c r="P9" s="2" t="str">
-        <f>O16</f>
-        <v xml:space="preserve"> 0.3530</v>
-      </c>
-      <c r="R9" s="4">
-        <v>8</v>
-      </c>
-      <c r="S9" s="3">
-        <f t="shared" si="5"/>
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="T9" s="3">
-        <f t="shared" si="6"/>
-        <v>0.47720000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.8182       </v>
-      </c>
-      <c r="H10" s="2" t="str">
-        <f>G18</f>
-        <v xml:space="preserve"> 0.8528       </v>
-      </c>
-      <c r="J10" s="4">
-        <v>9</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" si="1"/>
-        <v>0.8528</v>
-      </c>
-      <c r="L10" s="3">
-        <f t="shared" si="2"/>
-        <v>0.74770000000000003</v>
-      </c>
-      <c r="N10" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.3944 Acc: 0.8182        </v>
-      </c>
-      <c r="O10" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.3944</v>
-      </c>
-      <c r="P10" s="2" t="str">
-        <f>O18</f>
-        <v xml:space="preserve"> 0.3388</v>
-      </c>
-      <c r="R10" s="4">
-        <v>9</v>
-      </c>
-      <c r="S10" s="3">
-        <f t="shared" si="5"/>
-        <v>0.33879999999999999</v>
-      </c>
-      <c r="T10" s="3">
-        <f t="shared" si="6"/>
-        <v>0.48880000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7617       </v>
-      </c>
-      <c r="H11" s="2" t="str">
-        <f>G20</f>
-        <v xml:space="preserve"> 0.8544       </v>
-      </c>
-      <c r="J11" s="4">
-        <v>10</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" si="1"/>
-        <v>0.85440000000000005</v>
-      </c>
-      <c r="L11" s="3">
-        <f t="shared" si="2"/>
-        <v>0.71960000000000002</v>
-      </c>
-      <c r="N11" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4395 Acc: 0.7617        </v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4395</v>
-      </c>
-      <c r="P11" s="2" t="str">
-        <f>O20</f>
-        <v xml:space="preserve"> 0.3311</v>
-      </c>
-      <c r="R11" s="4">
-        <v>10</v>
-      </c>
-      <c r="S11" s="3">
-        <f t="shared" si="5"/>
-        <v>0.33110000000000001</v>
-      </c>
-      <c r="T11" s="3">
-        <f t="shared" si="6"/>
-        <v>0.51990000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.8286       </v>
-      </c>
-      <c r="I12" s="2" t="str">
-        <f>G3</f>
-        <v xml:space="preserve"> 0.7150       </v>
-      </c>
-      <c r="N12" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.3776 Acc: 0.8286        </v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.3776</v>
-      </c>
-      <c r="Q12" s="2" t="str">
-        <f>O3</f>
-        <v xml:space="preserve"> 0.4535</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7477       </v>
-      </c>
-      <c r="I13" s="2" t="str">
-        <f>G5</f>
-        <v xml:space="preserve"> 0.7290       </v>
-      </c>
-      <c r="N13" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4538 Acc: 0.7477        </v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4538</v>
-      </c>
-      <c r="Q13" s="2" t="str">
-        <f>O5</f>
-        <v xml:space="preserve"> 0.4203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.8343       </v>
-      </c>
-      <c r="I14" s="2" t="str">
-        <f>G7</f>
-        <v xml:space="preserve"> 0.7430       </v>
-      </c>
-      <c r="N14" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.3676 Acc: 0.8343        </v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.3676</v>
-      </c>
-      <c r="Q14" s="2" t="str">
-        <f>O7</f>
-        <v xml:space="preserve"> 0.4180</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7570       </v>
-      </c>
-      <c r="I15" s="2" t="str">
-        <f>G9</f>
-        <v xml:space="preserve"> 0.7570       </v>
-      </c>
-      <c r="N15" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4657 Acc: 0.7570        </v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4657</v>
-      </c>
-      <c r="Q15" s="2" t="str">
-        <f>O9</f>
-        <v xml:space="preserve"> 0.4282</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.8399       </v>
-      </c>
-      <c r="I16" s="2" t="str">
-        <f>G11</f>
-        <v xml:space="preserve"> 0.7617       </v>
-      </c>
-      <c r="N16" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.3530 Acc: 0.8399        </v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.3530</v>
-      </c>
-      <c r="Q16" s="2" t="str">
-        <f>O11</f>
-        <v xml:space="preserve"> 0.4395</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7523       </v>
-      </c>
-      <c r="I17" s="2" t="str">
-        <f>G13</f>
-        <v xml:space="preserve"> 0.7477       </v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4772 Acc: 0.7523        </v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4772</v>
-      </c>
-      <c r="Q17" s="2" t="str">
-        <f>O13</f>
-        <v xml:space="preserve"> 0.4538</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.8528       </v>
-      </c>
-      <c r="I18" s="2" t="str">
-        <f>G15</f>
-        <v xml:space="preserve"> 0.7570       </v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.3388 Acc: 0.8528        </v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.3388</v>
-      </c>
-      <c r="Q18" s="2" t="str">
-        <f>O15</f>
-        <v xml:space="preserve"> 0.4657</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7477       </v>
-      </c>
-      <c r="I19" s="2" t="str">
-        <f>G17</f>
-        <v xml:space="preserve"> 0.7523       </v>
-      </c>
-      <c r="N19" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.4888 Acc: 0.7477        </v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.4888</v>
-      </c>
-      <c r="Q19" s="2" t="str">
-        <f>O17</f>
-        <v xml:space="preserve"> 0.4772</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.8544       </v>
-      </c>
-      <c r="I20" s="2" t="str">
-        <f>G19</f>
-        <v xml:space="preserve"> 0.7477       </v>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.3311 Acc: 0.8544        </v>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.3311</v>
-      </c>
-      <c r="Q20" s="2" t="str">
-        <f>O19</f>
-        <v xml:space="preserve"> 0.4888</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0.7196       </v>
-      </c>
-      <c r="I21" s="2" t="str">
-        <f>G21</f>
-        <v xml:space="preserve"> 0.7196       </v>
-      </c>
-      <c r="N21" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> 0.5199 Acc: 0.7196        </v>
-      </c>
-      <c r="O21" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> 0.5199</v>
-      </c>
-      <c r="Q21" s="2" t="str">
-        <f>O21</f>
-        <v xml:space="preserve"> 0.5199</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0F3B07-AAFA-46F0-8254-5693D6AC1D0A}">
-  <dimension ref="A1:T23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
@@ -19384,7 +16231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E037784F-345C-4CAE-9649-2C2EA8A085A9}">
   <dimension ref="A1:T23"/>
   <sheetViews>
@@ -20163,7 +17010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47CB19B-DB62-4973-AE38-0AD90CC72E21}">
   <dimension ref="A1:T23"/>
   <sheetViews>
@@ -20942,7 +17789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C8C669-DD1D-41EE-9A01-D0B53DC00919}">
   <dimension ref="A1:T23"/>
   <sheetViews>
@@ -20987,7 +17834,7 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="G2" s="2" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(A2,":",-1)," ",-1)</f>
@@ -21034,7 +17881,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="G3" s="2" t="str">
         <f t="shared" ref="G3:G21" si="0">_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(A3,":",-1)," ",-1)</f>
@@ -21081,7 +17928,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21128,7 +17975,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21175,7 +18022,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="1" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21222,7 +18069,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="G7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21269,7 +18116,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="1" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21316,7 +18163,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="1" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21363,7 +18210,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21410,7 +18257,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="1" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21457,7 +18304,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21482,7 +18329,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21507,7 +18354,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21532,7 +18379,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21557,7 +18404,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="1" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21582,7 +18429,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21607,7 +18454,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21632,7 +18479,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="1" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21657,7 +18504,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21682,7 +18529,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="1" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21707,12 +18554,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="1" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -21722,7 +18569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2433102E-D79A-4FFA-8BAB-F573E00A9A86}">
   <dimension ref="A1:T23"/>
   <sheetViews>
@@ -21741,7 +18588,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>22</v>
@@ -21770,7 +18617,7 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="G2" s="2" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(A2,":",-1)," ",-1)</f>
@@ -21817,7 +18664,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="G3" s="2" t="str">
         <f t="shared" ref="G3:G21" si="0">_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(A3,":",-1)," ",-1)</f>
@@ -21864,7 +18711,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21911,7 +18758,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -21958,7 +18805,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="1" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22005,7 +18852,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="G7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22052,7 +18899,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="1" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22099,7 +18946,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="1" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22146,7 +18993,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="1" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22193,7 +19040,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="1" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22240,7 +19087,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22265,7 +19112,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22290,7 +19137,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22315,7 +19162,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="1" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22340,7 +19187,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="1" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22365,7 +19212,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22390,7 +19237,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22415,7 +19262,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="1" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22440,7 +19287,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22465,7 +19312,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="1" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -22490,12 +19337,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="1" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>